<commit_message>
added population data to calculate cross-country comparisons
</commit_message>
<xml_diff>
--- a/data_files/miscData/pakistan_gdp.xlsx
+++ b/data_files/miscData/pakistan_gdp.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/DistributionalNationalAccounts-Pakistan/data_files/miscData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34835C57-321C-C749-BBAC-D1EDD075DD60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50FDE692-7465-CB41-81F0-50062A09F097}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <r>
       <rPr>
@@ -32,43 +32,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">mgdpro_999_i_PK
-</t>
+      <t>Percentile</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Gross domestic product
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Total population | Constant local | ppp | constant (2017)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Pakistan</t>
-    </r>
+  </si>
+  <si>
+    <t>pall</t>
   </si>
   <si>
     <t>Country Code</t>
@@ -125,10 +93,22 @@
     <t>WID.world computations using: [URL][URL_LINK]http://data.worldbank.org/[/URL_LINK][URL_TEXT]World Bank[/URL_TEXT][/URL]; [URL][URL_LINK]http://unstats.un.org/unsd/snaama/Introduction.asp[/URL_LINK][URL_TEXT]United Nations National Accounts Main Aggregates Database[/URL_TEXT][/URL]; [URL][URL_LINK]http://www.ggdc.net/maddison/other_books/Contours_World_Economy.pdf[/URL_LINK][URL_TEXT]Maddison, Angus (2007). Contours of the World Economy 1-2030 AD.[/URL_TEXT][/URL]; [URL][URL_LINK]http://www.imf.org/external/pubs/ft/weo/2018/01/weodata/index.aspx/[/URL_LINK][URL_TEXT]IMF World Economic Outlook (04/2018)[/URL_TEXT][/URL]; [URL][URL_LINK]http://www.imf.org/external/pubs/ft/weo/2018/01/weodata/index.aspx/[/URL_LINK][URL_TEXT]IMF World Economic Outlook (04/2018)[/URL_TEXT][/URL]</t>
   </si>
   <si>
+    <t>mgdpro_999_i_PK
+Gross domestic product
+Total population | Constant local | ppp | constant (2017)
+Pakistan</t>
+  </si>
+  <si>
     <t>gdp</t>
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>gdp_index_2005</t>
+  </si>
+  <si>
+    <t>gdp_index_2017</t>
   </si>
 </sst>
 </file>
@@ -195,14 +175,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,169 +523,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2000</v>
       </c>
-      <c r="B2" s="6">
+      <c r="C2" s="3">
         <v>16118876995584</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="D2">
+        <v>76.694800000000001</v>
+      </c>
+      <c r="E2">
+        <f>(D2/$D$19)</f>
+        <v>0.48635482465624691</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2001</v>
       </c>
-      <c r="B3" s="6">
+      <c r="C3" s="3">
         <v>16536536350720</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="D3">
+        <v>78.682100000000005</v>
+      </c>
+      <c r="E3">
+        <f>(D3/$D$19)</f>
+        <v>0.4989571515811409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>2002</v>
       </c>
-      <c r="B4" s="6">
+      <c r="C4" s="3">
         <v>17211469070336</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="D4">
+        <v>81.893500000000003</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E19" si="0">(D4/$D$19)</f>
+        <v>0.51932202486982637</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>2003</v>
       </c>
-      <c r="B5" s="6">
+      <c r="C5" s="3">
         <v>18282568482816</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="D5">
+        <v>86.989800000000002</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.55163986249239827</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>2004</v>
       </c>
-      <c r="B6" s="6">
+      <c r="C6" s="3">
         <v>19656588918784</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="D6">
+        <v>93.527500000000003</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.5930982395551867</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
         <v>2005</v>
       </c>
-      <c r="B7" s="6">
+      <c r="C7" s="3">
         <v>21016900272128</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.63414315528073206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>2006</v>
       </c>
-      <c r="B8" s="6">
+      <c r="C8" s="3">
         <v>22155093868544</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="D8">
+        <v>105.4156</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.66848581199811541</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>2007</v>
       </c>
-      <c r="B9" s="6">
+      <c r="C9" s="3">
         <v>22863767666688</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="D9">
+        <v>108.78749999999999</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.68986848505102638</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>2008</v>
       </c>
-      <c r="B10" s="6">
+      <c r="C10" s="3">
         <v>23401412427776</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="D10">
+        <v>111.34569999999999</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.70609113524941802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>2009</v>
       </c>
-      <c r="B11" s="6">
+      <c r="C11" s="3">
         <v>23897275629568</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="D11">
+        <v>113.705</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0.72105247471195633</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>2010</v>
       </c>
-      <c r="B12" s="6">
+      <c r="C12" s="3">
         <v>24438296805376</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="D12">
+        <v>116.27930000000001</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0.73737722195834832</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
         <v>2011</v>
       </c>
-      <c r="B13" s="6">
+      <c r="C13" s="3">
         <v>25185939881984</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="D13">
+        <v>119.8366</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>0.75993559642114983</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>2012</v>
       </c>
-      <c r="B14" s="6">
+      <c r="C14" s="3">
         <v>26189083181056</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="D14">
+        <v>124.6096</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>0.79020324922269913</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
         <v>2013</v>
       </c>
-      <c r="B15" s="6">
+      <c r="C15" s="3">
         <v>27380225671168</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="D15">
+        <v>130.27719999999999</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>0.8261439466913898</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
         <v>2014</v>
       </c>
-      <c r="B16" s="6">
+      <c r="C16" s="3">
         <v>28656025993216</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="D16">
+        <v>136.3475</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>0.86463833864639617</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17">
         <v>2015</v>
       </c>
-      <c r="B17" s="6">
+      <c r="C17" s="3">
         <v>30150032883712</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="D17">
+        <v>143.45609999999999</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.90971703898268219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>2016</v>
       </c>
-      <c r="B18" s="6">
+      <c r="C18" s="3">
         <v>31508494548992</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="D18">
+        <v>149.91980000000001</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.95070615011056303</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
         <v>2017</v>
       </c>
-      <c r="B19" s="6">
+      <c r="C19" s="3">
         <v>33142192734208</v>
+      </c>
+      <c r="D19">
+        <v>157.69309999999999</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -715,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -726,63 +897,63 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="256" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>